<commit_message>
Fixed length of stay cleaning
</commit_message>
<xml_diff>
--- a/BoSClean/length_of_stay.xlsx
+++ b/BoSClean/length_of_stay.xlsx
@@ -24461,7 +24461,11 @@
       <c r="D1144" t="n">
         <v>370</v>
       </c>
-      <c r="E1144" t="inlineStr"/>
+      <c r="E1144" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1145">
       <c r="A1145" s="2" t="n">
@@ -24478,7 +24482,11 @@
       <c r="D1145" t="n">
         <v>370</v>
       </c>
-      <c r="E1145" t="inlineStr"/>
+      <c r="E1145" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1146">
       <c r="A1146" s="2" t="n">
@@ -24495,7 +24503,11 @@
       <c r="D1146" t="n">
         <v>370</v>
       </c>
-      <c r="E1146" t="inlineStr"/>
+      <c r="E1146" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1147">
       <c r="A1147" s="2" t="n">
@@ -24512,7 +24524,11 @@
       <c r="D1147" t="n">
         <v>370</v>
       </c>
-      <c r="E1147" t="inlineStr"/>
+      <c r="E1147" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1148">
       <c r="A1148" s="2" t="n">
@@ -24529,7 +24545,11 @@
       <c r="D1148" t="n">
         <v>370</v>
       </c>
-      <c r="E1148" t="inlineStr"/>
+      <c r="E1148" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1149">
       <c r="A1149" s="2" t="n">
@@ -24546,7 +24566,11 @@
       <c r="D1149" t="n">
         <v>370</v>
       </c>
-      <c r="E1149" t="inlineStr"/>
+      <c r="E1149" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1150">
       <c r="A1150" s="2" t="n">
@@ -24563,7 +24587,11 @@
       <c r="D1150" t="n">
         <v>370</v>
       </c>
-      <c r="E1150" t="inlineStr"/>
+      <c r="E1150" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1151">
       <c r="A1151" s="2" t="n">
@@ -24580,7 +24608,11 @@
       <c r="D1151" t="n">
         <v>370</v>
       </c>
-      <c r="E1151" t="inlineStr"/>
+      <c r="E1151" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1152">
       <c r="A1152" s="2" t="n">
@@ -24597,7 +24629,11 @@
       <c r="D1152" t="n">
         <v>370</v>
       </c>
-      <c r="E1152" t="inlineStr"/>
+      <c r="E1152" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1153">
       <c r="A1153" s="2" t="n">
@@ -24614,7 +24650,11 @@
       <c r="D1153" t="n">
         <v>370</v>
       </c>
-      <c r="E1153" t="inlineStr"/>
+      <c r="E1153" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1154">
       <c r="A1154" s="2" t="n">
@@ -24631,7 +24671,11 @@
       <c r="D1154" t="n">
         <v>370</v>
       </c>
-      <c r="E1154" t="inlineStr"/>
+      <c r="E1154" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1155">
       <c r="A1155" s="2" t="n">
@@ -24648,7 +24692,11 @@
       <c r="D1155" t="n">
         <v>483</v>
       </c>
-      <c r="E1155" t="inlineStr"/>
+      <c r="E1155" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1156">
       <c r="A1156" s="2" t="n">
@@ -24665,7 +24713,11 @@
       <c r="D1156" t="n">
         <v>483</v>
       </c>
-      <c r="E1156" t="inlineStr"/>
+      <c r="E1156" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1157">
       <c r="A1157" s="2" t="n">
@@ -24682,7 +24734,11 @@
       <c r="D1157" t="n">
         <v>505</v>
       </c>
-      <c r="E1157" t="inlineStr"/>
+      <c r="E1157" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1158">
       <c r="A1158" s="2" t="n">
@@ -24699,7 +24755,11 @@
       <c r="D1158" t="n">
         <v>505</v>
       </c>
-      <c r="E1158" t="inlineStr"/>
+      <c r="E1158" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1159">
       <c r="A1159" s="2" t="n">
@@ -24716,7 +24776,11 @@
       <c r="D1159" t="n">
         <v>1367</v>
       </c>
-      <c r="E1159" t="inlineStr"/>
+      <c r="E1159" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1160">
       <c r="A1160" s="2" t="n">
@@ -24733,7 +24797,11 @@
       <c r="D1160" t="n">
         <v>1268</v>
       </c>
-      <c r="E1160" t="inlineStr"/>
+      <c r="E1160" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1161">
       <c r="A1161" s="2" t="n">
@@ -24750,7 +24818,11 @@
       <c r="D1161" t="n">
         <v>1268</v>
       </c>
-      <c r="E1161" t="inlineStr"/>
+      <c r="E1161" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1162">
       <c r="A1162" s="2" t="n">
@@ -24767,7 +24839,11 @@
       <c r="D1162" t="n">
         <v>1268</v>
       </c>
-      <c r="E1162" t="inlineStr"/>
+      <c r="E1162" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1163">
       <c r="A1163" s="2" t="n">
@@ -24784,7 +24860,11 @@
       <c r="D1163" t="n">
         <v>1268</v>
       </c>
-      <c r="E1163" t="inlineStr"/>
+      <c r="E1163" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1164">
       <c r="A1164" s="2" t="n">
@@ -24801,7 +24881,11 @@
       <c r="D1164" t="n">
         <v>1268</v>
       </c>
-      <c r="E1164" t="inlineStr"/>
+      <c r="E1164" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1165">
       <c r="A1165" s="2" t="n">
@@ -24818,7 +24902,11 @@
       <c r="D1165" t="n">
         <v>1268</v>
       </c>
-      <c r="E1165" t="inlineStr"/>
+      <c r="E1165" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1166">
       <c r="A1166" s="2" t="n">
@@ -24835,7 +24923,11 @@
       <c r="D1166" t="n">
         <v>1268</v>
       </c>
-      <c r="E1166" t="inlineStr"/>
+      <c r="E1166" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1167">
       <c r="A1167" s="2" t="n">
@@ -24852,7 +24944,11 @@
       <c r="D1167" t="n">
         <v>1271</v>
       </c>
-      <c r="E1167" t="inlineStr"/>
+      <c r="E1167" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1168">
       <c r="A1168" s="2" t="n">
@@ -24869,7 +24965,11 @@
       <c r="D1168" t="n">
         <v>1271</v>
       </c>
-      <c r="E1168" t="inlineStr"/>
+      <c r="E1168" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1169">
       <c r="A1169" s="2" t="n">
@@ -24886,7 +24986,11 @@
       <c r="D1169" t="n">
         <v>1271</v>
       </c>
-      <c r="E1169" t="inlineStr"/>
+      <c r="E1169" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1170">
       <c r="A1170" s="2" t="n">
@@ -24903,7 +25007,11 @@
       <c r="D1170" t="n">
         <v>1273</v>
       </c>
-      <c r="E1170" t="inlineStr"/>
+      <c r="E1170" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1171">
       <c r="A1171" s="2" t="n">
@@ -24920,7 +25028,11 @@
       <c r="D1171" t="n">
         <v>1273</v>
       </c>
-      <c r="E1171" t="inlineStr"/>
+      <c r="E1171" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1172">
       <c r="A1172" s="2" t="n">
@@ -24937,7 +25049,11 @@
       <c r="D1172" t="n">
         <v>1273</v>
       </c>
-      <c r="E1172" t="inlineStr"/>
+      <c r="E1172" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1173">
       <c r="A1173" s="2" t="n">
@@ -24954,7 +25070,11 @@
       <c r="D1173" t="n">
         <v>1287</v>
       </c>
-      <c r="E1173" t="inlineStr"/>
+      <c r="E1173" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1174">
       <c r="A1174" s="2" t="n">
@@ -24971,7 +25091,11 @@
       <c r="D1174" t="n">
         <v>1287</v>
       </c>
-      <c r="E1174" t="inlineStr"/>
+      <c r="E1174" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1175">
       <c r="A1175" s="2" t="n">
@@ -24988,7 +25112,11 @@
       <c r="D1175" t="n">
         <v>1293</v>
       </c>
-      <c r="E1175" t="inlineStr"/>
+      <c r="E1175" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1176">
       <c r="A1176" s="2" t="n">
@@ -25005,7 +25133,11 @@
       <c r="D1176" t="n">
         <v>1293</v>
       </c>
-      <c r="E1176" t="inlineStr"/>
+      <c r="E1176" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1177">
       <c r="A1177" s="2" t="n">
@@ -25022,7 +25154,11 @@
       <c r="D1177" t="n">
         <v>1304</v>
       </c>
-      <c r="E1177" t="inlineStr"/>
+      <c r="E1177" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1178">
       <c r="A1178" s="2" t="n">
@@ -25039,7 +25175,11 @@
       <c r="D1178" t="n">
         <v>1318</v>
       </c>
-      <c r="E1178" t="inlineStr"/>
+      <c r="E1178" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1179">
       <c r="A1179" s="2" t="n">
@@ -25056,7 +25196,11 @@
       <c r="D1179" t="n">
         <v>1318</v>
       </c>
-      <c r="E1179" t="inlineStr"/>
+      <c r="E1179" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1180">
       <c r="A1180" s="2" t="n">
@@ -25073,7 +25217,11 @@
       <c r="D1180" t="n">
         <v>1318</v>
       </c>
-      <c r="E1180" t="inlineStr"/>
+      <c r="E1180" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1181">
       <c r="A1181" s="2" t="n">
@@ -25090,7 +25238,11 @@
       <c r="D1181" t="n">
         <v>1318</v>
       </c>
-      <c r="E1181" t="inlineStr"/>
+      <c r="E1181" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1182">
       <c r="A1182" s="2" t="n">
@@ -25107,7 +25259,11 @@
       <c r="D1182" t="n">
         <v>1318</v>
       </c>
-      <c r="E1182" t="inlineStr"/>
+      <c r="E1182" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1183">
       <c r="A1183" s="2" t="n">
@@ -25124,7 +25280,11 @@
       <c r="D1183" t="n">
         <v>1318</v>
       </c>
-      <c r="E1183" t="inlineStr"/>
+      <c r="E1183" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1184">
       <c r="A1184" s="2" t="n">
@@ -25141,7 +25301,11 @@
       <c r="D1184" t="n">
         <v>1337</v>
       </c>
-      <c r="E1184" t="inlineStr"/>
+      <c r="E1184" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1185">
       <c r="A1185" s="2" t="n">
@@ -25158,7 +25322,11 @@
       <c r="D1185" t="n">
         <v>1337</v>
       </c>
-      <c r="E1185" t="inlineStr"/>
+      <c r="E1185" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1186">
       <c r="A1186" s="2" t="n">
@@ -25175,7 +25343,11 @@
       <c r="D1186" t="n">
         <v>1337</v>
       </c>
-      <c r="E1186" t="inlineStr"/>
+      <c r="E1186" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1187">
       <c r="A1187" s="2" t="n">
@@ -25192,7 +25364,11 @@
       <c r="D1187" t="n">
         <v>874</v>
       </c>
-      <c r="E1187" t="inlineStr"/>
+      <c r="E1187" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1188">
       <c r="A1188" s="2" t="n">
@@ -25209,7 +25385,11 @@
       <c r="D1188" t="n">
         <v>874</v>
       </c>
-      <c r="E1188" t="inlineStr"/>
+      <c r="E1188" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1189">
       <c r="A1189" s="2" t="n">
@@ -25226,7 +25406,11 @@
       <c r="D1189" t="n">
         <v>874</v>
       </c>
-      <c r="E1189" t="inlineStr"/>
+      <c r="E1189" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1190">
       <c r="A1190" s="2" t="n">
@@ -25243,7 +25427,11 @@
       <c r="D1190" t="n">
         <v>1367</v>
       </c>
-      <c r="E1190" t="inlineStr"/>
+      <c r="E1190" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1191">
       <c r="A1191" s="2" t="n">
@@ -25260,7 +25448,11 @@
       <c r="D1191" t="n">
         <v>1367</v>
       </c>
-      <c r="E1191" t="inlineStr"/>
+      <c r="E1191" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1192">
       <c r="A1192" s="2" t="n">
@@ -25277,7 +25469,11 @@
       <c r="D1192" t="n">
         <v>1367</v>
       </c>
-      <c r="E1192" t="inlineStr"/>
+      <c r="E1192" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1193">
       <c r="A1193" s="2" t="n">
@@ -25294,7 +25490,11 @@
       <c r="D1193" t="n">
         <v>1367</v>
       </c>
-      <c r="E1193" t="inlineStr"/>
+      <c r="E1193" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1194">
       <c r="A1194" s="2" t="n">
@@ -25311,7 +25511,11 @@
       <c r="D1194" t="n">
         <v>1367</v>
       </c>
-      <c r="E1194" t="inlineStr"/>
+      <c r="E1194" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1195">
       <c r="A1195" s="2" t="n">
@@ -25328,7 +25532,11 @@
       <c r="D1195" t="n">
         <v>1367</v>
       </c>
-      <c r="E1195" t="inlineStr"/>
+      <c r="E1195" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1196">
       <c r="A1196" s="2" t="n">
@@ -25345,7 +25553,11 @@
       <c r="D1196" t="n">
         <v>1367</v>
       </c>
-      <c r="E1196" t="inlineStr"/>
+      <c r="E1196" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1197">
       <c r="A1197" s="2" t="n">
@@ -25362,7 +25574,11 @@
       <c r="D1197" t="n">
         <v>1378</v>
       </c>
-      <c r="E1197" t="inlineStr"/>
+      <c r="E1197" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1198">
       <c r="A1198" s="2" t="n">
@@ -25379,7 +25595,11 @@
       <c r="D1198" t="n">
         <v>1378</v>
       </c>
-      <c r="E1198" t="inlineStr"/>
+      <c r="E1198" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1199">
       <c r="A1199" s="2" t="n">
@@ -25396,7 +25616,11 @@
       <c r="D1199" t="n">
         <v>1380</v>
       </c>
-      <c r="E1199" t="inlineStr"/>
+      <c r="E1199" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1200">
       <c r="A1200" s="2" t="n">
@@ -25413,7 +25637,11 @@
       <c r="D1200" t="n">
         <v>1380</v>
       </c>
-      <c r="E1200" t="inlineStr"/>
+      <c r="E1200" t="inlineStr">
+        <is>
+          <t>Erin Park</t>
+        </is>
+      </c>
     </row>
     <row r="1201">
       <c r="A1201" s="2" t="n">

</xml_diff>